<commit_message>
add date formats to split-workbook
</commit_message>
<xml_diff>
--- a/pso-xlsx-core/src/test/resources/org/pageseeder/xlsx/core/dates/dates-sample.xlsx
+++ b/pso-xlsx-core/src/test/resources/org/pageseeder/xlsx/core/dates/dates-sample.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspace\berlioz\xlsx\pso-xlsx-core\src\test\resources\org\pageseeder\xlsx\core\dates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspace\pageseeder\xlsx\pso-xlsx-core\src\test\resources\org\pageseeder\xlsx\core\dates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3494DA8C-08C7-4BA1-8BCA-FFBB6E2CC9EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D5D634B-F868-4E8C-AA84-645A8C071B95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Default 14</t>
   </si>
@@ -53,16 +53,26 @@
   </si>
   <si>
     <t>The 14 format is 'MM/DD/YY' however it should be replaced by 'DD/MM/YY' as this is the format in Australia</t>
+  </si>
+  <si>
+    <t>D/M/YYYY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="10">
     <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="yyyy/mm/dd;@"/>
-    <numFmt numFmtId="167" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="167" formatCode="d/m/yyyy;@"/>
+    <numFmt numFmtId="168" formatCode="d/mm/yy;@"/>
+    <numFmt numFmtId="169" formatCode="d/m/yy;@"/>
+    <numFmt numFmtId="171" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="172" formatCode="[$-C09]dd\-mmm\-yy;@"/>
+    <numFmt numFmtId="173" formatCode="[$-C09]dd\-mmmm\-yyyy;@"/>
+    <numFmt numFmtId="174" formatCode="[$-C09]d\ mmmm\ yyyy;@"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -550,13 +560,20 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -912,10 +929,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59421F19-4F7D-4B30-9942-C4F8E6261F76}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1013,11 +1030,51 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="6">
+        <v>32</v>
+      </c>
+      <c r="C7" s="6">
+        <v>60</v>
+      </c>
+      <c r="D7" s="6">
+        <v>44228</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="7">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="8">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="9">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="10">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="11">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="12">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add month and year date formats to split-workbook
</commit_message>
<xml_diff>
--- a/pso-xlsx-core/src/test/resources/org/pageseeder/xlsx/core/dates/dates-sample.xlsx
+++ b/pso-xlsx-core/src/test/resources/org/pageseeder/xlsx/core/dates/dates-sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspace\pageseeder\xlsx\pso-xlsx-core\src\test\resources\org\pageseeder\xlsx\core\dates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D5D634B-F868-4E8C-AA84-645A8C071B95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9647CC8B-AD63-4BBB-88F2-B91830F6AB0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,11 +16,12 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" refMode="R1C1"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Default 14</t>
   </si>
@@ -56,23 +57,47 @@
   </si>
   <si>
     <t>D/M/YYYY</t>
+  </si>
+  <si>
+    <t>D/MM/YY</t>
+  </si>
+  <si>
+    <t>D/M/YY</t>
+  </si>
+  <si>
+    <t>DD/MM/YY</t>
+  </si>
+  <si>
+    <t>DD-MONTH-YYYY</t>
+  </si>
+  <si>
+    <t>DD-MON-YY</t>
+  </si>
+  <si>
+    <t>D Month YYYY</t>
+  </si>
+  <si>
+    <t>MM/DD/YY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="10">
+  <numFmts count="13">
     <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="yyyy/mm/dd;@"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="167" formatCode="d/m/yyyy;@"/>
     <numFmt numFmtId="168" formatCode="d/mm/yy;@"/>
     <numFmt numFmtId="169" formatCode="d/m/yy;@"/>
-    <numFmt numFmtId="171" formatCode="dd/mm/yy;@"/>
-    <numFmt numFmtId="172" formatCode="[$-C09]dd\-mmm\-yy;@"/>
-    <numFmt numFmtId="173" formatCode="[$-C09]dd\-mmmm\-yyyy;@"/>
-    <numFmt numFmtId="174" formatCode="[$-C09]d\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="170" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="171" formatCode="[$-C09]dd\-mmm\-yy;@"/>
+    <numFmt numFmtId="172" formatCode="[$-C09]dd\-mmmm\-yyyy;@"/>
+    <numFmt numFmtId="173" formatCode="[$-C09]d\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="179" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="180" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="181" formatCode="yy/mm/dd;@"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -560,7 +585,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -570,10 +595,13 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -929,15 +957,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59421F19-4F7D-4B30-9942-C4F8E6261F76}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
     <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.85546875" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
@@ -1044,34 +1072,81 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
       <c r="B8" s="7">
         <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
       <c r="B9" s="8">
         <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
       <c r="B10" s="9">
         <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
       <c r="B11" s="10">
         <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
       <c r="B12" s="11">
         <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
       <c r="B13" s="12">
         <v>32</v>
       </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="13">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="14">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update DatesTest (RichTextTrue) to assert new date and time formats
</commit_message>
<xml_diff>
--- a/pso-xlsx-core/src/test/resources/org/pageseeder/xlsx/core/dates/dates-sample.xlsx
+++ b/pso-xlsx-core/src/test/resources/org/pageseeder/xlsx/core/dates/dates-sample.xlsx
@@ -1,27 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspace\pageseeder\xlsx\pso-xlsx-core\src\test\resources\org\pageseeder\xlsx\core\dates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9647CC8B-AD63-4BBB-88F2-B91830F6AB0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BE8C406-8377-4CD9-BE75-C96026796996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15816" yWindow="2580" windowWidth="11136" windowHeight="9024" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" refMode="R1C1"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Default 14</t>
   </si>
@@ -78,13 +77,40 @@
   </si>
   <si>
     <t>MM/DD/YY</t>
+  </si>
+  <si>
+    <t>YYYY-MM-DD</t>
+  </si>
+  <si>
+    <t>YY-MM-DD</t>
+  </si>
+  <si>
+    <t>D/M/YY hh:mm AM/PM</t>
+  </si>
+  <si>
+    <t>D/M/YY hh:mm</t>
+  </si>
+  <si>
+    <t>hh:mm:ss AM/PM</t>
+  </si>
+  <si>
+    <t>hh:mm:ss</t>
+  </si>
+  <si>
+    <t>String formatted as date</t>
+  </si>
+  <si>
+    <t>I am a string that wants to be a date</t>
+  </si>
+  <si>
+    <t>h:mm:ss</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="13">
+  <numFmts count="19">
     <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="yyyy/mm/dd;@"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
@@ -95,9 +121,15 @@
     <numFmt numFmtId="171" formatCode="[$-C09]dd\-mmm\-yy;@"/>
     <numFmt numFmtId="172" formatCode="[$-C09]dd\-mmmm\-yyyy;@"/>
     <numFmt numFmtId="173" formatCode="[$-C09]d\ mmmm\ yyyy;@"/>
-    <numFmt numFmtId="179" formatCode="mm/dd/yy;@"/>
-    <numFmt numFmtId="180" formatCode="yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="181" formatCode="yy/mm/dd;@"/>
+    <numFmt numFmtId="174" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="175" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="176" formatCode="yy/mm/dd;@"/>
+    <numFmt numFmtId="177" formatCode="hh:mm:ss;@"/>
+    <numFmt numFmtId="178" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="179" formatCode="m/d/yy\ h:mm;@"/>
+    <numFmt numFmtId="180" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="181" formatCode="h:mm:ss;@"/>
+    <numFmt numFmtId="182" formatCode="d/mm/yyyy;@"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -585,7 +617,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -599,9 +631,16 @@
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -957,22 +996,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59421F19-4F7D-4B30-9942-C4F8E6261F76}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="96.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.44140625" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.88671875" customWidth="1"/>
+    <col min="4" max="4" width="33.88671875" customWidth="1"/>
+    <col min="5" max="5" width="96.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>4</v>
       </c>
@@ -986,7 +1025,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1003,7 +1042,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1018,7 +1057,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1032,7 +1071,7 @@
         <v>44228</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1046,7 +1085,7 @@
         <v>44228</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1057,7 +1096,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1071,7 +1110,7 @@
         <v>44228</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1079,47 +1118,57 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="8">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="9">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="10">
         <v>32</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="11">
         <v>32</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="12">
         <v>32</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1127,26 +1176,77 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
       <c r="B15" s="14">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
       <c r="B16" s="15">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
       <c r="B17" s="2">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="18">
+        <v>10.041666666666666</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="19">
+        <v>44403.000011574077</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="20">
+        <v>44403.000694444447</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="21">
+        <v>44403.042372685188</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="17">
+        <v>44403.48541666667</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>